<commit_message>
Component name changed-but still testing
having issues with 'calibration_result.py', 'calibration_result_dtss.py', 'validation_result.py', 'validation_result_dtss.py'.  couldn't reproduce the results as before, initial Q is weird, troubleshooting now
</commit_message>
<xml_diff>
--- a/exposan/pm2_ecorecover/data/initial_conditions_pm2_dynamic_influent_cali.xlsx
+++ b/exposan/pm2_ecorecover/data/initial_conditions_pm2_dynamic_influent_cali.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Downloads\EXPOsan\exposan\pm2_ecorecover\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54487720-99F1-4A73-B00C-AA3CB67B8D37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1987DAD7-E474-4669-831B-5CB1FFF20D2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" xr2:uid="{32702723-0D76-4F6C-A6A7-E56FCE88CE75}"/>
   </bookViews>
@@ -39,19 +39,10 @@
     <t>X_ALG</t>
   </si>
   <si>
-    <t>X_CH</t>
-  </si>
-  <si>
-    <t>X_LI</t>
-  </si>
-  <si>
     <t>S_CO2</t>
   </si>
   <si>
     <t>S_A</t>
-  </si>
-  <si>
-    <t>S_F</t>
   </si>
   <si>
     <t>S_O2</t>
@@ -79,6 +70,18 @@
   </si>
   <si>
     <t>MEV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X_PG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X_TAG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S_G</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -444,7 +447,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:N5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -457,22 +460,22 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -481,18 +484,18 @@
         <v>0</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2">
         <v>2.52985814982596</v>
@@ -536,7 +539,7 @@
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
         <v>2.52985814982596</v>
@@ -580,7 +583,7 @@
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2">
         <v>4.1742659472128336</v>
@@ -624,7 +627,7 @@
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>3.1724421198817541</v>

</xml_diff>